<commit_message>
vault backup: 2025-12-10 10:42:25
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F1BB29-6195-4398-A4CF-A9CAC48240E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013DDF17-F549-4497-AA7E-F72404D1C496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20676" yWindow="0" windowWidth="20424" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
+    <workbookView xWindow="10152" yWindow="0" windowWidth="18816" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
   <si>
     <t>Giocatore</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>Banca</t>
+  </si>
+  <si>
+    <t>THAC0 - CA avversario = Tiro necessario</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -573,48 +576,49 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -952,7 +956,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,13 +1042,13 @@
       <c r="B4" s="20">
         <v>4</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="29" t="s">
         <v>80</v>
       </c>
       <c r="K4" s="20">
@@ -1077,20 +1081,20 @@
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="K6" s="40" t="s">
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="K6" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
       <c r="N6" s="6">
         <v>10</v>
       </c>
@@ -1102,20 +1106,20 @@
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="K7" s="40" t="s">
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="K7" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
       <c r="N7" s="6">
         <v>10</v>
       </c>
@@ -1127,20 +1131,20 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="K8" s="40" t="s">
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="K8" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
       <c r="N8" s="6">
         <v>10</v>
       </c>
@@ -1152,20 +1156,20 @@
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="K9" s="40" t="s">
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="K9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
       <c r="N9" s="6">
         <v>13</v>
       </c>
@@ -1177,20 +1181,20 @@
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="K10" s="40" t="s">
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="K10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
       <c r="N10" s="6">
         <v>11</v>
       </c>
@@ -1202,15 +1206,15 @@
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
     </row>
     <row r="12" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1236,34 +1240,34 @@
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="30"/>
+      <c r="B14" s="36"/>
       <c r="E14" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="H14" s="32" t="s">
+      <c r="H14" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I14" s="32"/>
+      <c r="I14" s="40"/>
       <c r="L14" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
       <c r="E15" s="27" t="s">
         <v>79</v>
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="26"/>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="37">
         <v>11</v>
       </c>
       <c r="L15" s="8" t="s">
@@ -1271,16 +1275,16 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
       <c r="E16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="40">
         <v>12</v>
       </c>
       <c r="L16" s="8" t="s">
@@ -1288,17 +1292,17 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
       <c r="E17" s="27" t="s">
         <v>72</v>
       </c>
       <c r="F17" s="27"/>
       <c r="G17" s="26"/>
-      <c r="H17" s="33" t="s">
+      <c r="H17" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="37" t="s">
         <v>29</v>
       </c>
       <c r="L17" s="8" t="s">
@@ -1310,10 +1314,10 @@
         <v>73</v>
       </c>
       <c r="F18" s="7"/>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="40" t="s">
         <v>29</v>
       </c>
       <c r="L18" s="8" t="s">
@@ -1332,10 +1336,10 @@
       </c>
       <c r="F19" s="27"/>
       <c r="G19" s="26"/>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="I19" s="33"/>
+      <c r="I19" s="37"/>
       <c r="L19" s="8" t="s">
         <v>48</v>
       </c>
@@ -1355,14 +1359,17 @@
       <c r="A21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
+      <c r="E21" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
     </row>
     <row r="22" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
     </row>
     <row r="23" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
@@ -1382,10 +1389,10 @@
       <c r="B24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
       <c r="L24" s="3" t="s">
         <v>58</v>
       </c>
@@ -1397,10 +1404,10 @@
       <c r="B25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
       <c r="L25" s="3" t="s">
         <v>59</v>
       </c>
@@ -1409,10 +1416,10 @@
       <c r="A26" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
       <c r="L26" s="3" t="s">
         <v>60</v>
       </c>
@@ -1426,7 +1433,7 @@
       <c r="A28" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="37">
+      <c r="B28" s="32">
         <v>20</v>
       </c>
       <c r="C28" s="11"/>
@@ -1434,7 +1441,7 @@
       <c r="E28" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="36">
+      <c r="H28" s="31">
         <v>3</v>
       </c>
       <c r="L28" s="3" t="s">
@@ -1445,11 +1452,11 @@
       <c r="A29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="38">
+      <c r="B29" s="33">
         <v>5</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -1459,15 +1466,15 @@
       <c r="A30" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="38">
+      <c r="B30" s="33">
         <v>10</v>
       </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
     </row>
     <row r="31" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -1679,11 +1686,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A14:B17"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="L21:N21"/>
     <mergeCell ref="L22:N22"/>
     <mergeCell ref="C11:I11"/>
     <mergeCell ref="H18:I18"/>
@@ -1699,6 +1701,11 @@
     <mergeCell ref="C8:I8"/>
     <mergeCell ref="C9:I9"/>
     <mergeCell ref="C10:I10"/>
+    <mergeCell ref="A14:B17"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="L21:N21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-16 02:13:23
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5849A470-A00D-4085-B724-713879FA7E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841928C8-8922-41A7-92FC-49D550C8426B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10572" yWindow="0" windowWidth="23244" windowHeight="16656" activeTab="1" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
+    <workbookView xWindow="10572" yWindow="0" windowWidth="23244" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Scheda" sheetId="1" r:id="rId1"/>
+    <sheet name="Cleric" sheetId="1" r:id="rId1"/>
     <sheet name="Oggetti" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="117">
   <si>
     <t>Giocatore</t>
   </si>
@@ -79,24 +79,6 @@
   </si>
   <si>
     <t>Soffio Drago</t>
-  </si>
-  <si>
-    <t>EQUIPAGGIAMENTO</t>
-  </si>
-  <si>
-    <t>cotta di maglia e scudo</t>
-  </si>
-  <si>
-    <t>spada</t>
-  </si>
-  <si>
-    <t>2 pugnali</t>
-  </si>
-  <si>
-    <t>arco lungo</t>
-  </si>
-  <si>
-    <t>libro incantesimi</t>
   </si>
   <si>
     <t>open stuck doors on
@@ -109,9 +91,6 @@
     <t>Pietrificazione Paralisi</t>
   </si>
   <si>
-    <t>Veleno, Raggio della Morte</t>
-  </si>
-  <si>
     <t>Arma</t>
   </si>
   <si>
@@ -124,9 +103,6 @@
     <t>Correre</t>
   </si>
   <si>
-    <t>11km</t>
-  </si>
-  <si>
     <t>Spada</t>
   </si>
   <si>
@@ -137,9 +113,6 @@
   </si>
   <si>
     <t>Combattimento</t>
-  </si>
-  <si>
-    <t>Elf, Common, Chaotic, Orc, Hobgoblin, Gnoll, Gnome.</t>
   </si>
   <si>
     <t>Giornaliero</t>
@@ -183,12 +156,6 @@
     <t>1d6</t>
   </si>
   <si>
-    <t>cintura, stivali</t>
-  </si>
-  <si>
-    <t>abiti standard</t>
-  </si>
-  <si>
     <t>-1 on NPC reactions, max. 3 retainers, retainer morale 6</t>
   </si>
   <si>
@@ -198,36 +165,15 @@
     <t>1 Livello</t>
   </si>
   <si>
-    <t>Leggere magico, Scudo</t>
-  </si>
-  <si>
     <t>2 Livello</t>
   </si>
   <si>
-    <t>Invisibilità, Ragnatela</t>
-  </si>
-  <si>
-    <t>Infravisione 60piedi</t>
-  </si>
-  <si>
-    <t>2/6 trovare porte segrete</t>
-  </si>
-  <si>
     <t>1/6 Ascoltare rumori</t>
   </si>
   <si>
-    <t>1/6 ascoltare att. Porte</t>
-  </si>
-  <si>
-    <t>Immune paralisi Ghoul</t>
-  </si>
-  <si>
     <t>5 / 1/0/-1</t>
   </si>
   <si>
-    <t>Fast Character</t>
-  </si>
-  <si>
     <t>4th</t>
   </si>
   <si>
@@ -237,39 +183,18 @@
     <t>Elfo</t>
   </si>
   <si>
-    <t>Caotico</t>
-  </si>
-  <si>
-    <t>30.000/32,000</t>
-  </si>
-  <si>
     <t>Esperienza</t>
   </si>
   <si>
-    <t>6m / 4q</t>
-  </si>
-  <si>
     <t>Arrampicarsi</t>
   </si>
   <si>
     <t>Nuotare</t>
   </si>
   <si>
-    <t>18m / 12q</t>
-  </si>
-  <si>
-    <t>3m / 2q</t>
-  </si>
-  <si>
-    <t>19 km</t>
-  </si>
-  <si>
     <t>Peso</t>
   </si>
   <si>
-    <t>Pesante</t>
-  </si>
-  <si>
     <t>Esplorazione</t>
   </si>
   <si>
@@ -291,9 +216,6 @@
     <t>Incantesimi Scelti</t>
   </si>
   <si>
-    <t>Monete</t>
-  </si>
-  <si>
     <t>pp</t>
   </si>
   <si>
@@ -309,9 +231,6 @@
     <t>Slot</t>
   </si>
   <si>
-    <t>Anelli, amuleti, pergamene singole, chiavi</t>
-  </si>
-  <si>
     <t>Forza</t>
   </si>
   <si>
@@ -354,32 +273,135 @@
     <t>36+</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Esempio</t>
   </si>
   <si>
-    <t>Formula: 20 + (modificatore FOR × 2)</t>
-  </si>
-  <si>
     <t>Note/Usi/Cariche</t>
   </si>
   <si>
-    <t>Armi medie, armatura leggera, scudo , arco corto, balestra l.</t>
-  </si>
-  <si>
     <t>Armi grandi, armatura pesante, scudo grande, arco l., balestra p.</t>
   </si>
   <si>
-    <t>Ogni 100 mo</t>
-  </si>
-  <si>
-    <t>Armi piccole, torce, pozioni, corda, faretra</t>
+    <t>Armi piccole, torce, pozioni, corda, faretra, acqua s., bacchette</t>
+  </si>
+  <si>
+    <t>Armi m., armature l., scudo , arco c., balestra l., stivali, mantello</t>
+  </si>
+  <si>
+    <t>Anelli, amuleti, pergamene (10), chiavi, gemme</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Sutan Ambermoor</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>Neutrale</t>
+  </si>
+  <si>
+    <t>Veleno, Raggio della Morte, +1 mg</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>1/6 trovare porte segrete</t>
+  </si>
+  <si>
+    <t>1/6 ascoltare attr. Porte</t>
+  </si>
+  <si>
+    <t>Slot/Equipaggiamento</t>
+  </si>
+  <si>
+    <t>3/Armatura a piastre</t>
+  </si>
+  <si>
+    <t>1/Mazza</t>
+  </si>
+  <si>
+    <t>1/Fionda</t>
+  </si>
+  <si>
+    <t>0/Vestiti, Cintura, Stivali</t>
+  </si>
+  <si>
+    <t>0/Simbolo sacro</t>
+  </si>
+  <si>
+    <t>0/Fiale Acqua santa (2)</t>
+  </si>
+  <si>
+    <t>2/Scudo +1</t>
+  </si>
+  <si>
+    <t>Ogni 100 mo 1 Slot, Borsa Conservante +5 slot, fiale 1 slot ogni 5</t>
+  </si>
+  <si>
+    <t>Monete. 100=1slot</t>
+  </si>
+  <si>
+    <t>+6</t>
+  </si>
+  <si>
+    <t>4 Livello</t>
+  </si>
+  <si>
+    <t>Arma Potenziata +1d6</t>
+  </si>
+  <si>
+    <t>Benedizione +1TxC, Silenzio 5m</t>
+  </si>
+  <si>
+    <t>Cura Ferite Leggere 1d6+1, Protezione dal Male -1TxC</t>
+  </si>
+  <si>
+    <t>Cura Ferite Gravi  2d6+2</t>
+  </si>
+  <si>
+    <t>Piedi</t>
+  </si>
+  <si>
+    <t>Metri</t>
+  </si>
+  <si>
+    <t>Quad.</t>
+  </si>
+  <si>
+    <t>19km</t>
+  </si>
+  <si>
+    <t>12 mi</t>
+  </si>
+  <si>
+    <t>1R</t>
+  </si>
+  <si>
+    <t>1T</t>
+  </si>
+  <si>
+    <t>1G</t>
+  </si>
+  <si>
+    <t>Scacciare 2d6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +512,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
@@ -519,6 +548,20 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="6"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -562,7 +605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -582,21 +625,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -742,10 +770,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -834,25 +863,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -860,78 +883,126 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
@@ -1027,6 +1098,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1374,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263CECC3-3302-44DA-8376-3DD3643BBD45}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1400,12 +1488,12 @@
       <c r="G1" s="10"/>
       <c r="H1" s="8"/>
       <c r="I1" s="7" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
-      <c r="L1" s="10" t="s">
-        <v>66</v>
+      <c r="L1" s="68" t="s">
+        <v>86</v>
       </c>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
@@ -1415,15 +1503,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="9" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="8"/>
@@ -1433,7 +1521,7 @@
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="15" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
@@ -1459,22 +1547,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>75</v>
+        <v>50</v>
+      </c>
+      <c r="F4" s="30">
+        <v>20</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>102</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="20">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="K4" s="69">
+        <v>-1</v>
       </c>
       <c r="M4" s="16">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="N4" s="12" t="s">
         <v>10</v>
@@ -1483,7 +1574,7 @@
     </row>
     <row r="5" spans="1:15" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B5" s="14"/>
       <c r="K5" s="14" t="s">
@@ -1495,102 +1586,102 @@
     </row>
     <row r="6" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="K6" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="C6" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="K6" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
       <c r="N6" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="K7" s="40" t="s">
+      <c r="C7" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="K7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
       <c r="N7" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="K8" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
+      <c r="C8" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="K8" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
       <c r="N8" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="K9" s="40" t="s">
+      <c r="C9" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="K9" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
       <c r="N9" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1600,283 +1691,353 @@
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="K10" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
+      <c r="C10" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="K10" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
       <c r="N10" s="6">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
     </row>
     <row r="12" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="7"/>
-      <c r="E13" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="D13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="J13" s="75" t="s">
+        <v>110</v>
+      </c>
       <c r="K13" s="7"/>
       <c r="L13" s="9" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="9"/>
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="35"/>
-      <c r="E14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="H14" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" s="39"/>
+      <c r="A14" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="70"/>
+      <c r="D14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="G14" s="72" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" s="76">
+        <v>20</v>
+      </c>
+      <c r="I14" s="77">
+        <v>6</v>
+      </c>
+      <c r="J14" s="77">
+        <f>H14/5</f>
+        <v>4</v>
+      </c>
       <c r="L14" s="8" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="E15" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" s="36">
-        <v>11</v>
+      <c r="A15" s="70"/>
+      <c r="B15" s="70"/>
+      <c r="D15" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="79" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" s="80">
+        <v>60</v>
+      </c>
+      <c r="I15" s="80">
+        <v>18</v>
+      </c>
+      <c r="J15" s="80">
+        <f t="shared" ref="J15:J18" si="0">H15/5</f>
+        <v>12</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="E16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="H16" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="I16" s="39">
+      <c r="A16" s="70"/>
+      <c r="B16" s="70"/>
+      <c r="D16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="G16" s="72" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" s="76">
+        <v>60</v>
+      </c>
+      <c r="I16" s="77">
+        <v>18</v>
+      </c>
+      <c r="J16" s="77">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="E17" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="36" t="s">
-        <v>28</v>
+      <c r="A17" s="70"/>
+      <c r="B17" s="70"/>
+      <c r="D17" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="79" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" s="80">
+        <v>10</v>
+      </c>
+      <c r="I17" s="80">
+        <v>3</v>
+      </c>
+      <c r="J17" s="80">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="H18" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="39" t="s">
-        <v>28</v>
+      <c r="D18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="G18" s="72" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" s="76">
+        <v>10</v>
+      </c>
+      <c r="I18" s="77">
+        <v>3</v>
+      </c>
+      <c r="J18" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="B19" s="9"/>
-      <c r="E19" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" s="36"/>
+      <c r="D19" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="79" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="J19" s="78"/>
       <c r="L19" s="8" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="1">
+        <v>58</v>
+      </c>
+      <c r="B20" s="71">
         <v>0</v>
       </c>
-      <c r="L20" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="L20" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
     </row>
     <row r="21" spans="1:14" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="1">
-        <v>100</v>
-      </c>
-      <c r="E21" t="s">
-        <v>79</v>
-      </c>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
+        <v>55</v>
+      </c>
+      <c r="B21" s="71">
+        <v>500</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="M21" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="N21" s="72">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="1">
+        <v>59</v>
+      </c>
+      <c r="B22" s="71">
         <v>0</v>
       </c>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="N22" s="72">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="1">
+        <v>56</v>
+      </c>
+      <c r="B23" s="71">
         <v>0</v>
       </c>
-      <c r="L23" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
+      <c r="M23" s="73"/>
+      <c r="N23" s="81"/>
     </row>
     <row r="24" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L24" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73"/>
     </row>
     <row r="25" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B25" s="9"/>
-      <c r="L25" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="L25" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
     </row>
     <row r="26" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
+        <v>106</v>
+      </c>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
       <c r="L26" s="3" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
+        <v>105</v>
+      </c>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
       <c r="L27" s="3" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
+        <v>53</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
       <c r="L28" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
     <row r="31" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D32" s="22">
         <v>8</v>
@@ -1886,46 +2047,46 @@
         <v>7</v>
       </c>
       <c r="F32" s="22">
-        <f t="shared" ref="F32:L32" si="0">E32-1</f>
+        <f t="shared" ref="F32:L32" si="1">E32-1</f>
         <v>6</v>
       </c>
       <c r="G32" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H32" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I32" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J32" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K32" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L32" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M32" s="19" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="N32" s="19" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>29</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>38</v>
       </c>
       <c r="C33" s="24">
         <v>7</v>
@@ -1935,172 +2096,166 @@
         <v>8</v>
       </c>
       <c r="E33" s="24">
-        <f t="shared" ref="E33:L33" si="1">D33+1</f>
+        <f t="shared" ref="E33:L33" si="2">D33+1</f>
         <v>9</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G33" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="I33" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="J33" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="K33" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="L33" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M33" s="21" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="N33" s="1"/>
     </row>
     <row r="34" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C34" s="24">
         <v>8</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" ref="D34:L34" si="2">C34+1</f>
+        <f t="shared" ref="D34:L34" si="3">C34+1</f>
         <v>9</v>
       </c>
       <c r="E34" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="F34" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G34" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="I34" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="J34" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="K34" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="L34" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="M34" s="21" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="N34" s="1"/>
     </row>
     <row r="35" spans="1:27" ht="18" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C35" s="24">
         <v>9</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" ref="D35:L35" si="3">C35+1</f>
+        <f t="shared" ref="D35:L35" si="4">C35+1</f>
         <v>10</v>
       </c>
       <c r="E35" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="F35" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="G35" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="I35" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="J35" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="K35" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="L35" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="M35" s="21" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="AA36"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="L22:N22"/>
+  <mergeCells count="13">
     <mergeCell ref="C11:I11"/>
-    <mergeCell ref="H18:I18"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="K8:M8"/>
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="K10:M10"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H16:I16"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C8:I8"/>
     <mergeCell ref="C9:I9"/>
     <mergeCell ref="C10:I10"/>
     <mergeCell ref="A14:B17"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="L20:N20"/>
   </mergeCells>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
@@ -2110,8 +2265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7F733B-4F29-4CC7-8875-78DA591CD6C7}">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2124,57 +2279,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="A1" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="1:10" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="60">
+      <c r="A3" s="57">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
     </row>
     <row r="4" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="61">
+      <c r="A4" s="58">
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="62">
+      <c r="A5" s="59">
         <v>3</v>
       </c>
       <c r="B5"/>
@@ -2183,21 +2338,21 @@
       <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="61">
+      <c r="A6" s="58">
         <v>4</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="62">
+      <c r="A7" s="59">
         <v>5</v>
       </c>
       <c r="B7"/>
@@ -2206,21 +2361,21 @@
       <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="61">
+      <c r="A8" s="58">
         <v>6</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="62">
+      <c r="A9" s="59">
         <v>7</v>
       </c>
       <c r="B9"/>
@@ -2229,21 +2384,21 @@
       <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="61">
+      <c r="A10" s="58">
         <v>8</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62">
+      <c r="A11" s="59">
         <v>9</v>
       </c>
       <c r="B11"/>
@@ -2252,49 +2407,49 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63">
+      <c r="A12" s="60">
         <v>10</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
     </row>
     <row r="13" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="64">
+      <c r="A13" s="61">
         <v>11</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="33"/>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
     </row>
     <row r="14" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="65">
+      <c r="A14" s="62">
         <v>12</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
     </row>
     <row r="15" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="66">
+      <c r="A15" s="63">
         <v>13</v>
       </c>
       <c r="B15"/>
@@ -2303,21 +2458,21 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="61">
+      <c r="A16" s="58">
         <v>14</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="66">
+      <c r="A17" s="63">
         <v>15</v>
       </c>
       <c r="B17"/>
@@ -2326,21 +2481,21 @@
       <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="61">
+      <c r="A18" s="58">
         <v>16</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="66">
+      <c r="A19" s="63">
         <v>17</v>
       </c>
       <c r="B19"/>
@@ -2349,21 +2504,21 @@
       <c r="G19" s="34"/>
     </row>
     <row r="20" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="61">
+      <c r="A20" s="58">
         <v>18</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="66">
+      <c r="A21" s="63">
         <v>19</v>
       </c>
       <c r="B21"/>
@@ -2372,49 +2527,49 @@
       <c r="G21" s="34"/>
     </row>
     <row r="22" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="63">
+      <c r="A22" s="60">
         <v>20</v>
       </c>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
     </row>
     <row r="23" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="66">
+      <c r="A23" s="63">
         <v>21</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
       <c r="E23" s="33"/>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
     </row>
     <row r="24" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="65">
+      <c r="A24" s="62">
         <v>22</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="66">
+      <c r="A25" s="63">
         <v>23</v>
       </c>
       <c r="B25"/>
@@ -2423,21 +2578,21 @@
       <c r="G25" s="34"/>
     </row>
     <row r="26" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="61">
+      <c r="A26" s="58">
         <v>24</v>
       </c>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
     </row>
     <row r="27" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="66">
+      <c r="A27" s="63">
         <v>25</v>
       </c>
       <c r="B27"/>
@@ -2446,21 +2601,21 @@
       <c r="G27" s="34"/>
     </row>
     <row r="28" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="61">
+      <c r="A28" s="58">
         <v>26</v>
       </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="66">
+      <c r="A29" s="63">
         <v>27</v>
       </c>
       <c r="B29"/>
@@ -2469,71 +2624,71 @@
       <c r="G29" s="34"/>
     </row>
     <row r="30" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="61">
+      <c r="A30" s="58">
         <v>28</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="67">
+      <c r="A31" s="64">
         <v>29</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="H33" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="I33" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="J33" s="54" t="s">
-        <v>92</v>
+      <c r="A33" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="I33" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="J33" s="51" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>0</v>
       </c>
-      <c r="B34" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="69"/>
+      <c r="B34" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="66"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="52">
-        <v>3</v>
+      <c r="G34" s="67" t="s">
+        <v>84</v>
       </c>
       <c r="H34" s="1">
         <v>14</v>
@@ -2542,22 +2697,22 @@
         <v>4</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="68" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="69"/>
+      <c r="B35" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="66"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="52" t="s">
-        <v>93</v>
+      <c r="G35" s="49" t="s">
+        <v>66</v>
       </c>
       <c r="H35" s="1">
         <v>18</v>
@@ -2566,22 +2721,22 @@
         <v>5</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2</v>
       </c>
-      <c r="B36" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="69"/>
+      <c r="B36" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="66"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="52" t="s">
-        <v>94</v>
+      <c r="G36" s="49" t="s">
+        <v>67</v>
       </c>
       <c r="H36" s="1">
         <v>20</v>
@@ -2590,22 +2745,22 @@
         <v>6</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>3</v>
       </c>
-      <c r="B37" s="68" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="69"/>
+      <c r="B37" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="66"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="52" t="s">
-        <v>95</v>
+      <c r="G37" s="49" t="s">
+        <v>68</v>
       </c>
       <c r="H37" s="1">
         <v>22</v>
@@ -2614,22 +2769,22 @@
         <v>7</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>1</v>
-      </c>
-      <c r="B38" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="69"/>
+      <c r="A38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="66"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="52" t="s">
-        <v>96</v>
+      <c r="G38" s="49" t="s">
+        <v>69</v>
       </c>
       <c r="H38" s="1">
         <v>24</v>
@@ -2638,20 +2793,18 @@
         <v>8</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="A39" s="3"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="52" t="s">
-        <v>97</v>
+      <c r="G39" s="49" t="s">
+        <v>70</v>
       </c>
       <c r="H39" s="1">
         <v>26</v>
@@ -2660,7 +2813,7 @@
         <v>9</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-18 10:03:14
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13FF9D7-CFD2-4699-8AD5-DE74D9AD05F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042CB0E5-FAA0-4539-935C-DDD191052179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="0" windowWidth="27396" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
+    <workbookView xWindow="9888" yWindow="0" windowWidth="27396" windowHeight="16656" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Halfling A" sheetId="8" r:id="rId1"/>
@@ -2466,7 +2466,7 @@
   <dimension ref="A1:AA40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
vault backup: 2025-12-19 02:43:22
</commit_message>
<xml_diff>
--- a/Strumenti/Schede_DnD_BX91.xlsx
+++ b/Strumenti/Schede_DnD_BX91.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\Strumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785E4C04-EE58-447A-AE63-01E31F193E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FF27FC-1539-4027-B7CD-5AC961E36CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12216" yWindow="0" windowWidth="24120" windowHeight="16656" activeTab="8" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
+    <workbookView xWindow="12216" yWindow="0" windowWidth="24120" windowHeight="16656" activeTab="5" xr2:uid="{FC328CB3-F1C2-4520-956D-C4D288DB9EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Halfling A" sheetId="8" r:id="rId1"/>
@@ -760,9 +760,6 @@
     <t>Trasportati</t>
   </si>
   <si>
-    <t>Copertura: Parziale -2 TxC | Totale -4 TxC</t>
-  </si>
-  <si>
     <t>Prone: +2 TxC nemici, metà mov per alzarsi</t>
   </si>
   <si>
@@ -1103,6 +1100,9 @@
   </si>
   <si>
     <t>"Compra ora, pentiti dopo. Se torni vivo, sconto del 10%."</t>
+  </si>
+  <si>
+    <t>Copertura: Parziale -2 TxC | Quasi Totale -4 TxC</t>
   </si>
 </sst>
 </file>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" s="42"/>
       <c r="N20" s="179" t="s">
@@ -3378,7 +3378,7 @@
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" s="28"/>
       <c r="E21" s="138" t="str">
@@ -3390,7 +3390,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="43"/>
       <c r="E22" s="138" t="str">
@@ -3407,7 +3407,7 @@
     </row>
     <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" s="28"/>
       <c r="E23" s="138" t="str">
@@ -3421,7 +3421,7 @@
     </row>
     <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="70" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B24" s="43"/>
       <c r="E24" s="138" t="str">
@@ -3439,7 +3439,7 @@
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="67" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B25" s="28"/>
       <c r="C25" s="170"/>
@@ -3473,12 +3473,12 @@
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B27" s="23"/>
       <c r="E27" s="138" t="str">
         <f>'Cleric A'!E27</f>
-        <v>Copertura: Parziale -2 TxC | Totale -4 TxC</v>
+        <v>Copertura: Parziale -2 TxC | Quasi Totale -4 TxC</v>
       </c>
       <c r="N27" s="172" t="s">
         <v>43</v>
@@ -4333,7 +4333,7 @@
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" s="42"/>
       <c r="N20" s="179" t="s">
@@ -4344,7 +4344,7 @@
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" s="28"/>
       <c r="E21" s="138" t="str">
@@ -4358,7 +4358,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="43"/>
       <c r="E22" s="138" t="str">
@@ -4376,7 +4376,7 @@
     </row>
     <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" s="28"/>
       <c r="E23" s="138" t="str">
@@ -4390,7 +4390,7 @@
     </row>
     <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="70" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B24" s="43"/>
       <c r="E24" s="138" t="str">
@@ -4408,7 +4408,7 @@
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="67" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B25" s="28"/>
       <c r="E25" s="138" t="str">
@@ -4440,12 +4440,12 @@
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B27" s="23"/>
       <c r="E27" s="138" t="str">
         <f>'Cleric A'!E27</f>
-        <v>Copertura: Parziale -2 TxC | Totale -4 TxC</v>
+        <v>Copertura: Parziale -2 TxC | Quasi Totale -4 TxC</v>
       </c>
       <c r="N27" s="141" t="s">
         <v>43</v>
@@ -5309,7 +5309,7 @@
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" s="42"/>
       <c r="N20" s="179" t="s">
@@ -5320,7 +5320,7 @@
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" s="28"/>
       <c r="E21" s="138" t="str">
@@ -5332,7 +5332,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="43"/>
       <c r="E22" s="138" t="str">
@@ -5349,7 +5349,7 @@
     </row>
     <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" s="28"/>
       <c r="E23" s="138" t="str">
@@ -5363,7 +5363,7 @@
     </row>
     <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="70" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B24" s="43"/>
       <c r="E24" s="138" t="str">
@@ -5381,7 +5381,7 @@
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="67" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B25" s="28"/>
       <c r="E25" s="138" t="str">
@@ -5413,12 +5413,12 @@
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B27" s="23"/>
       <c r="E27" s="138" t="str">
         <f>'Cleric A'!E27</f>
-        <v>Copertura: Parziale -2 TxC | Totale -4 TxC</v>
+        <v>Copertura: Parziale -2 TxC | Quasi Totale -4 TxC</v>
       </c>
       <c r="N27" s="141" t="s">
         <v>43</v>
@@ -6295,7 +6295,7 @@
     </row>
     <row r="20" spans="1:21" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" s="42"/>
       <c r="N20" s="179" t="s">
@@ -6306,7 +6306,7 @@
     </row>
     <row r="21" spans="1:21" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" s="28"/>
       <c r="E21" s="138" t="str">
@@ -6318,7 +6318,7 @@
     </row>
     <row r="22" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="43"/>
       <c r="E22" s="138" t="str">
@@ -6336,7 +6336,7 @@
     </row>
     <row r="23" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" s="28"/>
       <c r="E23" s="138" t="str">
@@ -6351,7 +6351,7 @@
     </row>
     <row r="24" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="70" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B24" s="43"/>
       <c r="E24" s="138" t="str">
@@ -6371,7 +6371,7 @@
     </row>
     <row r="25" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="67" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B25" s="28"/>
       <c r="E25" s="138" t="str">
@@ -6407,12 +6407,12 @@
     </row>
     <row r="27" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B27" s="23"/>
       <c r="E27" s="138" t="str">
         <f>'Cleric A'!E27</f>
-        <v>Copertura: Parziale -2 TxC | Totale -4 TxC</v>
+        <v>Copertura: Parziale -2 TxC | Quasi Totale -4 TxC</v>
       </c>
       <c r="N27" s="141" t="s">
         <v>43</v>
@@ -6903,7 +6903,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="168" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -7299,7 +7299,7 @@
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" s="42"/>
       <c r="N20" s="179"/>
@@ -7308,7 +7308,7 @@
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" s="28"/>
       <c r="E21" s="138" t="str">
@@ -7320,7 +7320,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="43"/>
       <c r="E22" s="138" t="str">
@@ -7337,7 +7337,7 @@
     </row>
     <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" s="28"/>
       <c r="E23" s="138" t="str">
@@ -7351,7 +7351,7 @@
     </row>
     <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="70" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B24" s="43"/>
       <c r="E24" s="138" t="str">
@@ -7369,7 +7369,7 @@
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="67" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B25" s="28"/>
       <c r="E25" s="138" t="str">
@@ -7401,12 +7401,12 @@
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B27" s="23"/>
       <c r="E27" s="138" t="str">
         <f>'Cleric A'!E27</f>
-        <v>Copertura: Parziale -2 TxC | Totale -4 TxC</v>
+        <v>Copertura: Parziale -2 TxC | Quasi Totale -4 TxC</v>
       </c>
       <c r="N27" s="141" t="s">
         <v>43</v>
@@ -7765,8 +7765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D6BBBE-C9DF-4D21-98BF-29E96594E7D0}">
   <dimension ref="A1:AA40"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8269,7 +8269,7 @@
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" s="42"/>
       <c r="E20" s="138"/>
@@ -8281,7 +8281,7 @@
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" s="28"/>
       <c r="E21" s="138" t="str">
@@ -8293,7 +8293,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="43"/>
       <c r="E22" s="138" t="str">
@@ -8311,7 +8311,7 @@
     </row>
     <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" s="28"/>
       <c r="E23" s="138" t="str">
@@ -8324,7 +8324,7 @@
     </row>
     <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="70" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B24" s="43"/>
       <c r="E24" s="138" t="str">
@@ -8342,7 +8342,7 @@
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="67" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B25" s="28"/>
       <c r="E25" s="138" t="str">
@@ -8374,12 +8374,12 @@
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B27" s="23"/>
       <c r="E27" s="138" t="str">
         <f>'Cleric A'!E27</f>
-        <v>Copertura: Parziale -2 TxC | Totale -4 TxC</v>
+        <v>Copertura: Parziale -2 TxC | Quasi Totale -4 TxC</v>
       </c>
       <c r="N27" s="141" t="s">
         <v>43</v>
@@ -8748,8 +8748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263CECC3-3302-44DA-8376-3DD3643BBD45}">
   <dimension ref="A1:AA40"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9257,7 +9257,7 @@
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="93" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" s="92"/>
       <c r="N20" s="185" t="s">
@@ -9268,7 +9268,7 @@
     </row>
     <row r="21" spans="1:16" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="94" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" s="28"/>
       <c r="E21" s="138" t="s">
@@ -9280,7 +9280,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="95" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="43"/>
       <c r="E22" s="138" t="s">
@@ -9296,7 +9296,7 @@
     </row>
     <row r="23" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="94" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" s="28"/>
       <c r="E23" s="138" t="s">
@@ -9309,7 +9309,7 @@
     </row>
     <row r="24" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="95" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B24" s="43"/>
       <c r="E24" s="138" t="s">
@@ -9326,7 +9326,7 @@
     </row>
     <row r="25" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="94" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B25" s="28"/>
       <c r="E25" s="138" t="s">
@@ -9344,7 +9344,7 @@
       </c>
       <c r="B26" s="43"/>
       <c r="E26" s="142" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N26" s="141" t="s">
         <v>39</v>
@@ -9356,11 +9356,11 @@
     </row>
     <row r="27" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="96" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B27" s="23"/>
       <c r="E27" s="142" t="s">
-        <v>238</v>
+        <v>352</v>
       </c>
       <c r="N27" s="141" t="s">
         <v>43</v>
@@ -9371,7 +9371,7 @@
     <row r="28" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="63"/>
       <c r="E28" s="143" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N28" s="141" t="s">
         <v>40</v>
@@ -9383,7 +9383,7 @@
       <c r="A29" s="75"/>
       <c r="B29" s="23"/>
       <c r="E29" s="143" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N29" s="144"/>
       <c r="O29" s="139" t="s">
@@ -11012,7 +11012,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="100" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K37" s="98" t="s">
         <v>209</v>
@@ -11036,10 +11036,10 @@
     </row>
     <row r="38" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="99" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B38" s="110" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C38" s="111"/>
       <c r="D38" s="111"/>
@@ -11050,7 +11050,7 @@
       <c r="I38" s="111"/>
       <c r="J38" s="111"/>
       <c r="K38" s="107" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L38" s="108"/>
       <c r="M38" s="109">
@@ -11071,10 +11071,10 @@
     </row>
     <row r="39" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="99" t="s">
+        <v>251</v>
+      </c>
+      <c r="B39" s="112" t="s">
         <v>252</v>
-      </c>
-      <c r="B39" s="112" t="s">
-        <v>253</v>
       </c>
       <c r="K39" s="98" t="s">
         <v>210</v>
@@ -11101,7 +11101,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="110" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C40" s="110"/>
       <c r="D40" s="110"/>
@@ -11136,7 +11136,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="112" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K41" s="98" t="s">
         <v>212</v>
@@ -11163,7 +11163,7 @@
         <v>3</v>
       </c>
       <c r="B42" s="110" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C42" s="110"/>
       <c r="D42" s="110"/>
@@ -11225,7 +11225,7 @@
     </row>
     <row r="44" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B44" s="113"/>
       <c r="C44" s="19"/>
@@ -11237,7 +11237,7 @@
       <c r="I44" s="19"/>
       <c r="J44" s="3"/>
       <c r="K44" s="107" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L44" s="108"/>
       <c r="M44" s="109">
@@ -11258,7 +11258,7 @@
     </row>
     <row r="45" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B45" s="113"/>
       <c r="C45" s="19"/>
@@ -11285,7 +11285,7 @@
     </row>
     <row r="46" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B46" s="113"/>
       <c r="C46" s="19"/>
@@ -11297,7 +11297,7 @@
       <c r="I46" s="19"/>
       <c r="J46" s="3"/>
       <c r="K46" s="107" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L46" s="108"/>
       <c r="M46" s="109">
@@ -11307,14 +11307,14 @@
         <v>3</v>
       </c>
       <c r="O46" s="109" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P46" s="109"/>
       <c r="Q46" s="109"/>
     </row>
     <row r="47" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>
@@ -11388,8 +11388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7B6F9D-3ED0-4BE0-8E31-DC32197F8094}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11408,10 +11408,10 @@
         <v>45</v>
       </c>
       <c r="C1" s="198" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="198" t="s">
         <v>266</v>
-      </c>
-      <c r="D1" s="198" t="s">
-        <v>267</v>
       </c>
       <c r="E1" s="198" t="s">
         <v>46</v>
@@ -11425,13 +11425,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="199" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C2" s="196">
         <v>6</v>
       </c>
       <c r="D2" s="196" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E2" s="196">
         <v>1</v>
@@ -11443,19 +11443,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="199" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C3" s="196">
         <v>4</v>
       </c>
       <c r="D3" s="196" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E3" s="196">
         <v>1</v>
       </c>
       <c r="F3" s="195" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -11464,19 +11464,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="199" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C4" s="196">
         <v>10</v>
       </c>
       <c r="D4" s="196" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E4" s="196">
         <v>1</v>
       </c>
       <c r="F4" s="195" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -11485,19 +11485,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="199" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C5" s="196">
         <v>6</v>
       </c>
       <c r="D5" s="196" t="s">
+        <v>274</v>
+      </c>
+      <c r="E5" s="196" t="s">
+        <v>330</v>
+      </c>
+      <c r="F5" s="195" t="s">
         <v>275</v>
-      </c>
-      <c r="E5" s="196" t="s">
-        <v>331</v>
-      </c>
-      <c r="F5" s="195" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -11506,19 +11506,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="199" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C6" s="196">
         <v>4</v>
       </c>
       <c r="D6" s="196" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E6" s="196">
         <v>1</v>
       </c>
       <c r="F6" s="195" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -11527,19 +11527,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="199" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C7" s="196">
         <v>6</v>
       </c>
       <c r="D7" s="196" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E7" s="196">
         <v>0</v>
       </c>
       <c r="F7" s="195" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -11548,19 +11548,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="199" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C8" s="196">
         <v>6</v>
       </c>
       <c r="D8" s="196" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E8" s="196">
         <v>1</v>
       </c>
       <c r="F8" s="195" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -11569,13 +11569,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="199" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C9" s="196">
         <v>4</v>
       </c>
       <c r="D9" s="196" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E9" s="196">
         <v>1</v>
@@ -11587,19 +11587,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="199" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C10" s="196">
         <v>2</v>
       </c>
       <c r="D10" s="196" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E10" s="196">
         <v>1</v>
       </c>
       <c r="F10" s="195" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -11608,19 +11608,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="199" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C11" s="196">
         <v>10</v>
       </c>
       <c r="D11" s="196" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E11" s="196">
         <v>0</v>
       </c>
       <c r="F11" s="195" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -11629,19 +11629,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="199" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C12" s="196">
         <v>12</v>
       </c>
       <c r="D12" s="196" t="s">
+        <v>290</v>
+      </c>
+      <c r="E12" s="196" t="s">
+        <v>329</v>
+      </c>
+      <c r="F12" s="195" t="s">
         <v>291</v>
-      </c>
-      <c r="E12" s="196" t="s">
-        <v>330</v>
-      </c>
-      <c r="F12" s="195" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -11650,13 +11650,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="199" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C13" s="196">
         <v>8</v>
       </c>
       <c r="D13" s="196" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E13" s="196">
         <v>1</v>
@@ -11668,13 +11668,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="199" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C14" s="196">
         <v>6</v>
       </c>
       <c r="D14" s="196" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E14" s="196">
         <v>1</v>
@@ -11686,7 +11686,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="199" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C15" s="196">
         <v>10</v>
@@ -11704,19 +11704,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="199" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C16" s="196">
         <v>10</v>
       </c>
       <c r="D16" s="196" t="s">
+        <v>296</v>
+      </c>
+      <c r="E16" s="196" t="s">
+        <v>329</v>
+      </c>
+      <c r="F16" s="195" t="s">
         <v>297</v>
-      </c>
-      <c r="E16" s="196" t="s">
-        <v>330</v>
-      </c>
-      <c r="F16" s="195" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -11725,19 +11725,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="199" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C17" s="196">
         <v>6</v>
       </c>
       <c r="D17" s="196" t="s">
+        <v>299</v>
+      </c>
+      <c r="E17" s="196" t="s">
+        <v>329</v>
+      </c>
+      <c r="F17" s="195" t="s">
         <v>300</v>
-      </c>
-      <c r="E17" s="196" t="s">
-        <v>330</v>
-      </c>
-      <c r="F17" s="195" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -11746,19 +11746,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="199" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C18" s="196">
         <v>2</v>
       </c>
       <c r="D18" s="196" t="s">
+        <v>302</v>
+      </c>
+      <c r="E18" s="196" t="s">
+        <v>329</v>
+      </c>
+      <c r="F18" s="195" t="s">
         <v>303</v>
-      </c>
-      <c r="E18" s="196" t="s">
-        <v>330</v>
-      </c>
-      <c r="F18" s="195" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -11767,19 +11767,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="199" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C19" s="196">
         <v>2</v>
       </c>
       <c r="D19" s="196" t="s">
+        <v>305</v>
+      </c>
+      <c r="E19" s="196" t="s">
+        <v>329</v>
+      </c>
+      <c r="F19" s="195" t="s">
         <v>306</v>
-      </c>
-      <c r="E19" s="196" t="s">
-        <v>330</v>
-      </c>
-      <c r="F19" s="195" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -11788,19 +11788,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="199" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C20" s="196">
         <v>3</v>
       </c>
       <c r="D20" s="196" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E20" s="196" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F20" s="195" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -11809,16 +11809,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="199" t="s">
+        <v>335</v>
+      </c>
+      <c r="D21" s="196" t="s">
+        <v>302</v>
+      </c>
+      <c r="E21" s="196" t="s">
+        <v>329</v>
+      </c>
+      <c r="F21" s="195" t="s">
         <v>336</v>
-      </c>
-      <c r="D21" s="196" t="s">
-        <v>303</v>
-      </c>
-      <c r="E21" s="196" t="s">
-        <v>330</v>
-      </c>
-      <c r="F21" s="195" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -11827,19 +11827,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="199" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C22" s="196">
         <v>4</v>
       </c>
       <c r="D22" s="196" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E22" s="196" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F22" s="195" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -11848,19 +11848,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="199" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C23" s="196">
         <v>2</v>
       </c>
       <c r="D23" s="196" t="s">
+        <v>338</v>
+      </c>
+      <c r="E23" s="196" t="s">
+        <v>329</v>
+      </c>
+      <c r="F23" s="195" t="s">
         <v>339</v>
-      </c>
-      <c r="E23" s="196" t="s">
-        <v>330</v>
-      </c>
-      <c r="F23" s="195" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -11869,19 +11869,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="199" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C24" s="196">
         <v>3</v>
       </c>
       <c r="D24" s="196" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E24" s="196">
         <v>0</v>
       </c>
       <c r="F24" s="195" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -11890,19 +11890,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="199" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C25" s="196">
         <v>2</v>
       </c>
       <c r="D25" s="196" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E25" s="196">
         <v>0</v>
       </c>
       <c r="F25" s="195" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -11911,19 +11911,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="199" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C26" s="196">
         <v>2</v>
       </c>
       <c r="D26" s="196" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E26" s="196">
         <v>0</v>
       </c>
       <c r="F26" s="195" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -11932,19 +11932,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="199" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C27" s="196">
         <v>2</v>
       </c>
       <c r="D27" s="196" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E27" s="196">
         <v>0</v>
       </c>
       <c r="F27" s="195" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -11953,19 +11953,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="199" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C28" s="196">
         <v>1</v>
       </c>
       <c r="D28" s="196" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E28" s="196">
         <v>0</v>
       </c>
       <c r="F28" s="195" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -11974,19 +11974,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="199" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C29" s="196">
         <v>1</v>
       </c>
       <c r="D29" s="196" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E29" s="196">
         <v>0</v>
       </c>
       <c r="F29" s="195" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -11995,19 +11995,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="199" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C30" s="196">
         <v>4</v>
       </c>
       <c r="D30" s="196" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E30" s="196">
         <v>0</v>
       </c>
       <c r="F30" s="195" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -12016,19 +12016,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="199" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C31" s="196">
         <v>2</v>
       </c>
       <c r="D31" s="196" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E31" s="196">
         <v>0</v>
       </c>
       <c r="F31" s="195" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -12037,19 +12037,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="199" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C32" s="196">
         <v>3</v>
       </c>
       <c r="D32" s="196" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E32" s="196">
         <v>0</v>
       </c>
       <c r="F32" s="195" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -12058,19 +12058,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="199" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C33" s="196">
         <v>2</v>
       </c>
       <c r="D33" s="196" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E33" s="196">
         <v>0</v>
       </c>
       <c r="F33" s="195" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -12079,19 +12079,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="199" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C34" s="196">
         <v>2</v>
       </c>
       <c r="D34" s="196" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E34" s="196">
         <v>0</v>
       </c>
       <c r="F34" s="195" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="8.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12100,19 +12100,19 @@
         <v>40</v>
       </c>
       <c r="B36" s="201" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C36" s="202">
         <v>3</v>
       </c>
       <c r="D36" s="202" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E36" s="202">
         <v>0</v>
       </c>
       <c r="F36" s="203" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -12120,19 +12120,19 @@
         <v>41</v>
       </c>
       <c r="B37" s="199" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C37" s="196">
         <v>2</v>
       </c>
       <c r="D37" s="196" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E37" s="196">
         <v>0</v>
       </c>
       <c r="F37" s="195" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -12140,19 +12140,19 @@
         <v>42</v>
       </c>
       <c r="B38" s="201" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C38" s="202">
         <v>4</v>
       </c>
       <c r="D38" s="202" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E38" s="202">
         <v>0</v>
       </c>
       <c r="F38" s="203" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -12160,25 +12160,25 @@
         <v>43</v>
       </c>
       <c r="B39" s="199" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C39" s="196">
         <v>3</v>
       </c>
       <c r="D39" s="196" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E39" s="196">
         <v>1</v>
       </c>
       <c r="F39" s="195" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="200" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C41" s="200"/>
       <c r="D41" s="200"/>

</xml_diff>